<commit_message>
added file to read excel or csv into a data frame, also added code to split if/then into antecedent conseqence so that I can put into LegalRuleML
</commit_message>
<xml_diff>
--- a/PyDevShamroq/src/edu/ttu/acm/dataset-cfr_16_312_005.xlsx
+++ b/PyDevShamroq/src/edu/ttu/acm/dataset-cfr_16_312_005.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\PycharmProjects\research\PyDevShamroq\src\edu\ttu\acm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAB9EEF1-5AD3-49C0-B24E-CC71E82732F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EE4F54-92C8-48AA-AFD6-61DB3A6CB0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset-cfr_16_312_005" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'dataset-cfr_16_312_005'!$A$1:$G$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -511,7 +514,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -989,8 +992,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1345,36 +1357,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.77734375" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="88.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="79.109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1382,10 +1398,10 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1393,10 +1409,10 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1404,10 +1420,10 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1415,43 +1431,43 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1459,131 +1475,131 @@
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>41</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1591,10 +1607,10 @@
       <c r="A21" t="s">
         <v>44</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1602,65 +1618,65 @@
       <c r="A22" t="s">
         <v>47</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>50</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>53</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>56</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>56</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>60</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="5" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1668,32 +1684,32 @@
       <c r="A28" t="s">
         <v>63</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>66</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>66</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="5" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1701,10 +1717,10 @@
       <c r="A31" t="s">
         <v>70</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="5" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1712,10 +1728,10 @@
       <c r="A32" t="s">
         <v>70</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="5" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1723,87 +1739,87 @@
       <c r="A33" t="s">
         <v>70</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>75</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>75</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>75</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>80</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>83</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>86</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>86</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="5" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1811,175 +1827,175 @@
       <c r="A41" t="s">
         <v>90</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>93</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>93</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>97</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>97</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>97</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>102</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>102</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>106</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>106</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>110</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>110</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>110</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>110</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>116</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>119</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="5" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1987,10 +2003,10 @@
       <c r="A57" t="s">
         <v>122</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="5" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1998,10 +2014,10 @@
       <c r="A58" t="s">
         <v>122</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="5" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2009,10 +2025,10 @@
       <c r="A59" t="s">
         <v>122</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="5" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2020,10 +2036,10 @@
       <c r="A60" t="s">
         <v>122</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="5" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2031,10 +2047,10 @@
       <c r="A61" t="s">
         <v>122</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="5" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2042,10 +2058,10 @@
       <c r="A62" t="s">
         <v>122</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="5" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2053,10 +2069,10 @@
       <c r="A63" t="s">
         <v>122</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="5" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2064,10 +2080,10 @@
       <c r="A64" t="s">
         <v>122</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="5" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2075,10 +2091,10 @@
       <c r="A65" t="s">
         <v>132</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="5" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2086,10 +2102,10 @@
       <c r="A66" t="s">
         <v>132</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="5" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2097,10 +2113,10 @@
       <c r="A67" t="s">
         <v>132</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="5" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2108,10 +2124,10 @@
       <c r="A68" t="s">
         <v>137</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="5" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2119,65 +2135,65 @@
       <c r="A69" t="s">
         <v>140</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>143</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="5" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>146</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>146</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>146</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>146</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="5" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2185,10 +2201,10 @@
       <c r="A75" t="s">
         <v>152</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="5" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2196,21 +2212,21 @@
       <c r="A76" t="s">
         <v>152</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>156</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="5" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2218,14 +2234,16 @@
       <c r="A78" t="s">
         <v>159</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="5" t="s">
         <v>161</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>